<commit_message>
[CAN-56] fixed TFSM and RFSM requirements
</commit_message>
<xml_diff>
--- a/CAN_merge/Requirements/can_bitstream_processor_requirements.xlsx
+++ b/CAN_merge/Requirements/can_bitstream_processor_requirements.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\40010377\Documents\GitHub\CAN-Controller\CAN_merge\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B625B8A-AA7C-4638-9755-821BEBA436AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FB8435-DED6-4069-9A3C-14A8B26340D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Bit Timing Module" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -407,27 +406,9 @@
     <t>The Module shall initialize o_can_ready to logic low on system startup.</t>
   </si>
   <si>
-    <t>The Module shall set int_rstate_next equal to IFS when int_rstate is IDLE,  i_samp_tick is logic high, and int_rxbit_history[7:0] is 8'hFF.</t>
-  </si>
-  <si>
-    <t>The Module shall set int_rstate_next equal to BUSY when int_rstate is IFS, i_samp_tick is logic high, and int_rxbit_history[3:0] is 3'b1110.</t>
-  </si>
-  <si>
-    <t>The Module shall set int_rstate_next equal to IFS when int_rstate is BUSY, i_samp_tick is logic high, and int_rxbit_history[7:0] is 8'hFF.</t>
-  </si>
-  <si>
-    <t>The Module shall set int_tstate_next equal to IFS when int_tstate is IDLE, i_samp_tick is logic high, and int_txbit_history[7:0] is 8'hFF.</t>
-  </si>
-  <si>
-    <t>The Module shall set int_tstate_next equal to IDLE when int_tstate is IFS, i_samp_tick is logic high, and int_txbit_history[3:0] is 3'b1110.</t>
-  </si>
-  <si>
     <t>The Module shall set int_tstate_next equal to BUSY when int_tstate is IFS, i_samp_tick is logic high, int_txbit_history[2:0] is 3'b111, and i_send_en is logic high.</t>
   </si>
   <si>
-    <t>The Module shall set int_tstate_next equal to IFS when int_tstate is BUSY, i_samp_tick is logic high, and int_txbit_history[7:0] is 8'hFF.</t>
-  </si>
-  <si>
     <t>The Module shall set int_mstate_next equal to NORMAL when i_cen is logic high, i_reset is logic low, i_lback is logic low, and i_sleep is logic low.</t>
   </si>
   <si>
@@ -1191,6 +1172,24 @@
   </si>
   <si>
     <t>The Module shall set i_send_data[109:126] equal to int_rxframe_reg[13:30] when int_rstate is IFS and int_rxframe_reg[12] is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_tstate_next equal to IFS when int_tstate is BUSY, i_samp_tick is logic high, int_txbit_history[6:0] is 7'h7F, and o_tx_bit is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_tstate_next equal to IFS when int_tstate is IDLE, i_samp_tick is logic high, int_txbit_history[6:0] is 7'h7F, and o_tx_bit is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rstate_next equal to IFS when int_rstate is BUSY, i_samp_tick is logic high, and int_rxbit_history[6:0] is 7'h7F, and o_rx_bit is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rstate_next equal to IFS when int_rstate is IDLE,  i_samp_tick is logic high, int_rxbit_history[6:0] is 7'h7F, and i_rx_bit is logic high.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_rstate_next equal to BUSY when int_rstate is IFS, i_samp_tick is logic high, int_rxbit_history[2:0] is 3'b111, and i_rx_bit is logic low.</t>
+  </si>
+  <si>
+    <t>The Module shall set int_tstate_next equal to IDLE when int_tstate is IFS, i_samp_tick is logic high, int_rxbit_history[2:0] is 3'b111, and o_tx_bit is logic high.</t>
   </si>
 </sst>
 </file>
@@ -1984,8 +1983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C114" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="C69" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2545,7 +2544,7 @@
         <v>83</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2567,7 +2566,7 @@
         <v>95</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>132</v>
+        <v>382</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -2577,7 +2576,7 @@
         <v>96</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2587,7 +2586,7 @@
         <v>97</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>130</v>
+        <v>387</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2597,7 +2596,7 @@
         <v>98</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>129</v>
+        <v>383</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2619,7 +2618,7 @@
         <v>101</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>128</v>
+        <v>384</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2629,7 +2628,7 @@
         <v>102</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>127</v>
+        <v>386</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2639,871 +2638,871 @@
         <v>103</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>126</v>
+        <v>385</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="46"/>
       <c r="B64" s="42" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="D64" s="24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="46"/>
       <c r="B65" s="43"/>
       <c r="C65" s="9" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="46"/>
       <c r="B66" s="43"/>
       <c r="C66" s="20" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="46"/>
       <c r="B67" s="43"/>
       <c r="C67" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D67" s="13" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="46"/>
       <c r="B68" s="43"/>
       <c r="C68" s="20" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="46"/>
       <c r="B69" s="43"/>
       <c r="C69" s="9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="46"/>
       <c r="B70" s="43"/>
       <c r="C70" s="20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="46"/>
       <c r="B71" s="43"/>
       <c r="C71" s="9" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D71" s="13" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="46"/>
       <c r="B72" s="43"/>
       <c r="C72" s="20" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="46"/>
       <c r="B73" s="43"/>
       <c r="C73" s="9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="46"/>
       <c r="B74" s="43"/>
       <c r="C74" s="20" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D74" s="18" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="46"/>
       <c r="B75" s="43"/>
       <c r="C75" s="9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="46"/>
       <c r="B76" s="43"/>
       <c r="C76" s="20" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="46"/>
       <c r="B77" s="43"/>
       <c r="C77" s="9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="46"/>
       <c r="B78" s="43"/>
       <c r="C78" s="20" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="46"/>
       <c r="B79" s="43"/>
       <c r="C79" s="9" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D79" s="13" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="46"/>
       <c r="B80" s="43"/>
       <c r="C80" s="20" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="46"/>
       <c r="B81" s="47"/>
       <c r="C81" s="9" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D81" s="16" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="46"/>
       <c r="B82" s="53" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D82" s="24" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="46"/>
       <c r="B83" s="54"/>
       <c r="C83" s="9" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D83" s="13" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="46"/>
       <c r="B84" s="54"/>
       <c r="C84" s="20" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="46"/>
       <c r="B85" s="54"/>
       <c r="C85" s="9" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="D85" s="13" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="46"/>
       <c r="B86" s="54"/>
       <c r="C86" s="20" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="46"/>
       <c r="B87" s="54"/>
       <c r="C87" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="D87" s="13" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="46"/>
       <c r="B88" s="54"/>
       <c r="C88" s="20" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D88" s="18" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="46"/>
       <c r="B89" s="54"/>
       <c r="C89" s="9" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="46"/>
       <c r="B90" s="55"/>
       <c r="C90" s="25" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="46"/>
       <c r="B91" s="53" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="C91" s="21" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D91" s="22" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="46"/>
       <c r="B92" s="54"/>
       <c r="C92" s="20" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D92" s="18" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="46"/>
       <c r="B93" s="54"/>
       <c r="C93" s="9" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D93" s="13" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="46"/>
       <c r="B94" s="54"/>
       <c r="C94" s="20" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D94" s="18" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="46"/>
       <c r="B95" s="54"/>
       <c r="C95" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="46"/>
       <c r="B96" s="54"/>
       <c r="C96" s="20" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="46"/>
       <c r="B97" s="54"/>
       <c r="C97" s="9" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="46"/>
       <c r="B98" s="54"/>
       <c r="C98" s="20" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D98" s="18" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="46"/>
       <c r="B99" s="54"/>
       <c r="C99" s="9" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="46"/>
       <c r="B100" s="54"/>
       <c r="C100" s="20" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D100" s="18" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="46"/>
       <c r="B101" s="54"/>
       <c r="C101" s="11" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="46"/>
       <c r="B102" s="42" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C102" s="23" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="D102" s="24" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A103" s="46"/>
       <c r="B103" s="47"/>
       <c r="C103" s="11" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="D103" s="16" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="46"/>
       <c r="B104" s="42" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D104" s="24" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A105" s="46"/>
       <c r="B105" s="47"/>
       <c r="C105" s="11" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D105" s="16" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="46"/>
       <c r="B106" s="42" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C106" s="23" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="D106" s="24" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="46"/>
       <c r="B107" s="43"/>
       <c r="C107" s="9" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="46"/>
       <c r="B108" s="43"/>
       <c r="C108" s="20" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="D108" s="18" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="46"/>
       <c r="B109" s="43"/>
       <c r="C109" s="9" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="46"/>
       <c r="B110" s="43"/>
       <c r="C110" s="20" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="D110" s="18" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="46"/>
       <c r="B111" s="43"/>
       <c r="C111" s="9" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="46"/>
       <c r="B112" s="43"/>
       <c r="C112" s="20" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="D112" s="18" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="46"/>
       <c r="B113" s="43"/>
       <c r="C113" s="9" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="46"/>
       <c r="B114" s="43"/>
       <c r="C114" s="20" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="46"/>
       <c r="B115" s="43"/>
       <c r="C115" s="9" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="46"/>
       <c r="B116" s="43"/>
       <c r="C116" s="20" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D116" s="18" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="46"/>
       <c r="B117" s="43"/>
       <c r="C117" s="9" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D117" s="13" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="46"/>
       <c r="B118" s="43"/>
       <c r="C118" s="20" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="D118" s="18" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="46"/>
       <c r="B119" s="43"/>
       <c r="C119" s="9" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D119" s="13" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="46"/>
       <c r="B120" s="43"/>
       <c r="C120" s="20" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="D120" s="18" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="46"/>
       <c r="B121" s="43"/>
       <c r="C121" s="9" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D121" s="13" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="46"/>
       <c r="B122" s="43"/>
       <c r="C122" s="20" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D122" s="18" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="46"/>
       <c r="B123" s="43"/>
       <c r="C123" s="9" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="D123" s="13" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="46"/>
       <c r="B124" s="43"/>
       <c r="C124" s="20" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="46"/>
       <c r="B125" s="43"/>
       <c r="C125" s="9" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D125" s="13" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="46"/>
       <c r="B126" s="43"/>
       <c r="C126" s="20" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="46"/>
       <c r="B127" s="43"/>
       <c r="C127" s="9" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D127" s="13" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="46"/>
       <c r="B128" s="43"/>
       <c r="C128" s="20" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="46"/>
       <c r="B129" s="43"/>
       <c r="C129" s="9" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D129" s="13" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="46"/>
       <c r="B130" s="43"/>
       <c r="C130" s="20" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="D130" s="18" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="46"/>
       <c r="B131" s="43"/>
       <c r="C131" s="9" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="46"/>
       <c r="B132" s="43"/>
       <c r="C132" s="20" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="D132" s="18" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="46"/>
       <c r="B133" s="43"/>
       <c r="C133" s="9" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D133" s="13" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="46"/>
       <c r="B134" s="43"/>
       <c r="C134" s="20" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="D134" s="18" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="46"/>
       <c r="B135" s="43"/>
       <c r="C135" s="9" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="D135" s="13" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="46"/>
       <c r="B136" s="43"/>
       <c r="C136" s="20" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="D136" s="18" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="46"/>
       <c r="B137" s="43"/>
       <c r="C137" s="9" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="D137" s="13" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="46"/>
       <c r="B138" s="43"/>
       <c r="C138" s="20" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="D138" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="46"/>
       <c r="B139" s="43"/>
       <c r="C139" s="9" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="D139" s="13" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="46"/>
       <c r="B140" s="43"/>
       <c r="C140" s="20" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="D140" s="18" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="46"/>
       <c r="B141" s="43"/>
       <c r="C141" s="9" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="D141" s="13" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="46"/>
       <c r="B142" s="47"/>
       <c r="C142" s="28" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="D142" s="27" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="46"/>
       <c r="B143" s="42" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C143" s="21" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="46"/>
       <c r="B144" s="43"/>
       <c r="C144" s="20" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="D144" s="18" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="46"/>
       <c r="B145" s="43"/>
       <c r="C145" s="9" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="D145" s="13" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="46"/>
       <c r="B146" s="43"/>
       <c r="C146" s="20" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="D146" s="18" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="46"/>
       <c r="B147" s="43"/>
       <c r="C147" s="9" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="D147" s="13" t="s">
-        <v>290</v>
+        <v>284</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A148" s="46"/>
       <c r="B148" s="44"/>
       <c r="C148" s="25" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="D148" s="26" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -3560,46 +3559,46 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>293</v>
+        <v>287</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="51"/>
       <c r="C3" s="1" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="D3" s="34" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="49"/>
       <c r="B4" s="51"/>
       <c r="C4" s="9" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>296</v>
+        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="51"/>
       <c r="C5" s="1" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="H5" s="41"/>
       <c r="I5" s="41"/>
@@ -3611,10 +3610,10 @@
       <c r="A6" s="49"/>
       <c r="B6" s="51"/>
       <c r="C6" s="9" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="H6" s="41"/>
       <c r="I6" s="41"/>
@@ -3626,10 +3625,10 @@
       <c r="A7" s="49"/>
       <c r="B7" s="51"/>
       <c r="C7" s="1" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="H7" s="41"/>
       <c r="I7" s="41"/>
@@ -3641,10 +3640,10 @@
       <c r="A8" s="49"/>
       <c r="B8" s="52"/>
       <c r="C8" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="H8" s="41"/>
       <c r="I8" s="41"/>
@@ -3658,10 +3657,10 @@
         <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="D9" s="39" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="H9" s="41"/>
       <c r="I9" s="41"/>
@@ -3673,10 +3672,10 @@
       <c r="A10" s="49"/>
       <c r="B10" s="51"/>
       <c r="C10" s="9" t="s">
-        <v>300</v>
+        <v>294</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="H10" s="41"/>
       <c r="I10" s="41"/>
@@ -3688,10 +3687,10 @@
       <c r="A11" s="49"/>
       <c r="B11" s="51"/>
       <c r="C11" s="1" t="s">
-        <v>301</v>
+        <v>295</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>304</v>
+        <v>298</v>
       </c>
       <c r="H11" s="41"/>
       <c r="I11" s="41"/>
@@ -3703,10 +3702,10 @@
       <c r="A12" s="49"/>
       <c r="B12" s="51"/>
       <c r="C12" s="9" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
@@ -3718,10 +3717,10 @@
       <c r="A13" s="49"/>
       <c r="B13" s="51"/>
       <c r="C13" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
@@ -3733,254 +3732,254 @@
       <c r="A14" s="49"/>
       <c r="B14" s="51"/>
       <c r="C14" s="9" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49"/>
       <c r="B15" s="57"/>
       <c r="C15" s="31" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="D15" s="40" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="50" t="s">
-        <v>305</v>
+        <v>299</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="51"/>
       <c r="C17" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="D17" s="34" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="51"/>
       <c r="C18" s="9" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="D18" s="35" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="51"/>
       <c r="C19" s="1" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="51"/>
       <c r="C20" s="9" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="57"/>
       <c r="C21" s="31" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="50" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
       <c r="B23" s="51"/>
       <c r="C23" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D23" s="34" t="s">
         <v>318</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="51"/>
       <c r="C24" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="D24" s="35" t="s">
         <v>319</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="51"/>
       <c r="C25" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D25" s="34" t="s">
         <v>320</v>
-      </c>
-      <c r="D25" s="34" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="51"/>
       <c r="C26" s="9" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="51"/>
       <c r="C27" s="1" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="D27" s="34" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="51"/>
       <c r="C28" s="9" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
       <c r="B29" s="51"/>
       <c r="C29" s="1" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D29" s="34" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
       <c r="B30" s="51"/>
       <c r="C30" s="9" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="51"/>
       <c r="C31" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D31" s="34" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
       <c r="B32" s="51"/>
       <c r="C32" s="9" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
       <c r="B33" s="51"/>
       <c r="C33" s="1" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="D33" s="34" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="49"/>
       <c r="B34" s="51"/>
       <c r="C34" s="9" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="49"/>
       <c r="B35" s="51"/>
       <c r="C35" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="D35" s="34" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
       <c r="B36" s="51"/>
       <c r="C36" s="9" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
       <c r="B37" s="51"/>
       <c r="C37" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D37" s="34" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="56"/>
       <c r="B38" s="57"/>
       <c r="C38" s="36" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>